<commit_message>
feat: align tmux window/terminal tab switching behavior
</commit_message>
<xml_diff>
--- a/Settings/macOS/Keycodes WSL.xlsx
+++ b/Settings/macOS/Keycodes WSL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markus/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markus/Projects/wiki/Settings/macOS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A59AD5-BD96-5048-919E-00B3E202BD61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D6AEF0-E628-C54E-9019-ECC7F8637551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="76800" yWindow="500" windowWidth="25600" windowHeight="28300" xr2:uid="{50588C59-C901-4884-96BD-5BD174B20F9B}"/>
+    <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="28300" xr2:uid="{50588C59-C901-4884-96BD-5BD174B20F9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -618,7 +618,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -956,7 +956,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="236" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1128,13 +1128,13 @@
       <c r="E6" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="1" t="s">
         <v>68</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="3" t="s">
         <v>69</v>
       </c>
       <c r="I6" s="1" t="s">
@@ -1157,13 +1157,13 @@
       <c r="E7" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="1" t="s">
         <v>74</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="3" t="s">
         <v>75</v>
       </c>
       <c r="I7" s="1" t="s">

</xml_diff>